<commit_message>
Refine zabbix syslog check
</commit_message>
<xml_diff>
--- a/監視設定チェックシート_Zabbix.xlsx
+++ b/監視設定チェックシート_Zabbix.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="チェック対象" sheetId="1" r:id="rId1"/>
     <sheet name="監視設定チェックシート(Zabbix)" sheetId="2" r:id="rId2"/>
     <sheet name="検査ルール" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
   <si>
     <t>項目ID</t>
   </si>
@@ -235,10 +235,21 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Linux Syslog の取得サイズ。全ホスト検査の場合は未使用</t>
-  </si>
-  <si>
     <t>x &gt; 0</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Linux Syslog の取得サイズ。全ホスト検査の場合は別シートに登録</t>
+    <rPh sb="30" eb="31">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>トウロク</t>
+    </rPh>
     <phoneticPr fontId="6"/>
   </si>
 </sst>
@@ -291,6 +302,7 @@
     <font>
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -995,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1257,9 +1269,11 @@
       <c r="D16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="F16" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
@@ -1541,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1618,7 +1632,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="12"/>
     </row>

</xml_diff>